<commit_message>
Modificaciones ortografia y Select especialidad
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/Indicaciones/IndicacionesListado.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/Indicaciones/IndicacionesListado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\API\Service.Catalog\wwwroot\layout\excel\Indicaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1550EC-A965-47E2-A896-60955E039D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83DB0D4-42CB-4157-A0A6-9D470DC337FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Indicaciones" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Indicaciones">Indicaciones!$H$5+Indicaciones!$A$4:$D$5</definedName>
+    <definedName name="Indicaciones">Indicaciones!$A$4:$D$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -180,10 +180,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,7 +557,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,16 +571,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">

</xml_diff>